<commit_message>
Up vicuna question sbs
</commit_message>
<xml_diff>
--- a/sbs/vicuna_question_ru/openai_davinci_003_gusev_fred.xlsx
+++ b/sbs/vicuna_question_ru/openai_davinci_003_gusev_fred.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexkuk/proj/rulm-sbs/sbs/vicuna_question_ru/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E00A600-7826-D44E-A0AF-4F001074E5DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C77CED6-CE09-3248-A423-363C4A989AF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1715,8 +1715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E81"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="E60" sqref="E60"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1756,6 +1756,9 @@
       <c r="D2" s="2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" s="2">
+        <v>-2</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="335" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
@@ -1770,6 +1773,9 @@
       <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="E3" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="350" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
@@ -1784,6 +1790,9 @@
       <c r="D4" s="2" t="s">
         <v>13</v>
       </c>
+      <c r="E4" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="272" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
@@ -1798,6 +1807,9 @@
       <c r="D5" s="2" t="s">
         <v>16</v>
       </c>
+      <c r="E5" s="2">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="350" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
@@ -2730,6 +2742,9 @@
       <c r="D60" s="2" t="s">
         <v>181</v>
       </c>
+      <c r="E60" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="61" spans="1:5" ht="144" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
@@ -2744,6 +2759,9 @@
       <c r="D61" s="2" t="s">
         <v>184</v>
       </c>
+      <c r="E61" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="62" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A62" s="2">
@@ -2758,6 +2776,9 @@
       <c r="D62" s="2" t="s">
         <v>187</v>
       </c>
+      <c r="E62" s="2">
+        <v>-1</v>
+      </c>
     </row>
     <row r="63" spans="1:5" ht="272" x14ac:dyDescent="0.2">
       <c r="A63" s="2">
@@ -2772,6 +2793,9 @@
       <c r="D63" s="2" t="s">
         <v>190</v>
       </c>
+      <c r="E63" s="2">
+        <v>-2</v>
+      </c>
     </row>
     <row r="64" spans="1:5" ht="176" x14ac:dyDescent="0.2">
       <c r="A64" s="2">
@@ -2786,8 +2810,11 @@
       <c r="D64" s="2" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" ht="240" x14ac:dyDescent="0.2">
+      <c r="E64" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" ht="240" x14ac:dyDescent="0.2">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -2800,8 +2827,11 @@
       <c r="D65" s="2" t="s">
         <v>196</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="E65" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -2814,8 +2844,11 @@
       <c r="D66" s="2" t="s">
         <v>199</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" ht="272" x14ac:dyDescent="0.2">
+      <c r="E66" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" ht="272" x14ac:dyDescent="0.2">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -2828,8 +2861,11 @@
       <c r="D67" s="2" t="s">
         <v>202</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" ht="320" x14ac:dyDescent="0.2">
+      <c r="E67" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" ht="320" x14ac:dyDescent="0.2">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -2842,8 +2878,11 @@
       <c r="D68" s="2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="E68" s="2">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -2856,8 +2895,11 @@
       <c r="D69" s="2" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="E69" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -2870,8 +2912,11 @@
       <c r="D70" s="2" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" ht="48" x14ac:dyDescent="0.2">
+      <c r="E70" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" ht="48" x14ac:dyDescent="0.2">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -2884,8 +2929,11 @@
       <c r="D71" s="2" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="72" spans="1:4" ht="256" x14ac:dyDescent="0.2">
+      <c r="E71" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" ht="256" x14ac:dyDescent="0.2">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -2898,8 +2946,11 @@
       <c r="D72" s="2" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="73" spans="1:4" ht="208" x14ac:dyDescent="0.2">
+      <c r="E72" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" ht="208" x14ac:dyDescent="0.2">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -2912,8 +2963,11 @@
       <c r="D73" s="2" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="74" spans="1:4" ht="350" x14ac:dyDescent="0.2">
+      <c r="E73" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" ht="350" x14ac:dyDescent="0.2">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -2926,8 +2980,11 @@
       <c r="D74" s="2" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="75" spans="1:4" ht="350" x14ac:dyDescent="0.2">
+      <c r="E74" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" ht="350" x14ac:dyDescent="0.2">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -2940,8 +2997,11 @@
       <c r="D75" s="2" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="76" spans="1:4" ht="240" x14ac:dyDescent="0.2">
+      <c r="E75" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" ht="240" x14ac:dyDescent="0.2">
       <c r="A76" s="2">
         <v>75</v>
       </c>
@@ -2954,8 +3014,11 @@
       <c r="D76" s="2" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="77" spans="1:4" ht="409.6" x14ac:dyDescent="0.2">
+      <c r="E76" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" ht="409.6" x14ac:dyDescent="0.2">
       <c r="A77" s="2">
         <v>76</v>
       </c>
@@ -2968,8 +3031,11 @@
       <c r="D77" s="2" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="78" spans="1:4" ht="288" x14ac:dyDescent="0.2">
+      <c r="E77" s="2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" ht="288" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -2982,8 +3048,11 @@
       <c r="D78" s="2" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="79" spans="1:4" ht="272" x14ac:dyDescent="0.2">
+      <c r="E78" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" ht="272" x14ac:dyDescent="0.2">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -2996,8 +3065,11 @@
       <c r="D79" s="2" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="80" spans="1:4" ht="350" x14ac:dyDescent="0.2">
+      <c r="E79" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" ht="350" x14ac:dyDescent="0.2">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -3010,8 +3082,11 @@
       <c r="D80" s="2" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" ht="240" x14ac:dyDescent="0.2">
+      <c r="E80" s="2">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" ht="240" x14ac:dyDescent="0.2">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -3023,6 +3098,9 @@
       </c>
       <c r="D81" s="2" t="s">
         <v>244</v>
+      </c>
+      <c r="E81" s="2">
+        <v>-1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>